<commit_message>
Fixed the problem with the replication method
</commit_message>
<xml_diff>
--- a/ShopifyExcel/ShopifyExcel/wwwroot/Phil test 4.xlsx
+++ b/ShopifyExcel/ShopifyExcel/wwwroot/Phil test 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD58307A-CF13-4C9C-BB10-33214935783F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC659C7-6879-479D-9E47-945F613F618B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{95E89F0A-F415-4BFF-B0B0-52118C828AC5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Handle</t>
   </si>
@@ -108,10 +108,10 @@
     <t>Collection</t>
   </si>
   <si>
-    <t>4711 Perfume By Muelhens Deodorant Spray (Unisex)</t>
-  </si>
-  <si>
-    <t>100% Genuine 4711 Deodorant Spray (Unisex) By Muelhens 5 Oz</t>
+    <t>007 Cologne By James Bond Eau De Toilette Spray</t>
+  </si>
+  <si>
+    <t>100% Authentic 007 EDT Spray By James Bond 1 /2.7 /4.2 Oz</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -161,18 +161,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 Deodorant Spray (Unisex) By Muelhens 5 Oz
+                    100% Authentic 007 EDT Spray By James Bond 1 /2.7 /4.2 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
+                &lt;p&gt;007 Cologne by James Bond, A mysterious and alluring new cologne inspired by ian flemingâ€™s fictional character james bond is to be released in 2012. The launching of this secretive menâ€™s cologne is scheduled to coincide with the 50th anniversary of the first debut of the original film, as well as the release of the newest james bond movie. While there is yet no scoop on what this new cologne will smell like, it is certain to be as enchanting, alluring and mysterious as its inspiration.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/58258W.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/007JB1.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -244,7 +244,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -256,18 +255,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -278,16 +272,16 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>Muelhens</t>
-  </si>
-  <si>
-    <t>Deodorant Spray (Unisex)</t>
+    <t>James Bond</t>
+  </si>
+  <si>
+    <t>Eau De Toilette Spray</t>
   </si>
   <si>
     <t>Size</t>
   </si>
   <si>
-    <t>5 oz Deodorant Spray</t>
+    <t>1 oz Eau De Toilette Spray</t>
   </si>
   <si>
     <t>shopify</t>
@@ -299,19 +293,13 @@
     <t>manual</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/58258W.jpg</t>
-  </si>
-  <si>
-    <t>Perfume for Women</t>
-  </si>
-  <si>
-    <t>Perfume</t>
-  </si>
-  <si>
-    <t>4711 Cologne By Muelhens Eau De Cologne (Unisex)</t>
-  </si>
-  <si>
-    <t>100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz</t>
+    <t>https://img.fragrancex.com/images/products/SKU/large/007JB1.jpg</t>
+  </si>
+  <si>
+    <t>Cologne for Men</t>
+  </si>
+  <si>
+    <t>Cologne</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -361,18 +349,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Authentic 007 EDT Spray By James Bond 1 /2.7 /4.2 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
+                &lt;p&gt;007 Cologne by James Bond, A mysterious and alluring new cologne inspired by ian flemingâ€™s fictional character james bond is to be released in 2012. The launching of this secretive menâ€™s cologne is scheduled to coincide with the 50th anniversary of the first debut of the original film, as well as the release of the newest james bond movie. While there is yet no scoop on what this new cologne will smell like, it is certain to be as enchanting, alluring and mysterious as its inspiration.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C17.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/M71974JM.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -444,7 +432,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -456,18 +443,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -478,19 +460,10 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>Eau De Cologne (Unisex)</t>
-  </si>
-  <si>
-    <t>1.7 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/471C17.jpg</t>
-  </si>
-  <si>
-    <t>Cologne for Men</t>
-  </si>
-  <si>
-    <t>Cologne</t>
+    <t>2.7 oz Eau De Toilette Spray</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/M71974JM.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -540,18 +513,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Authentic 007 EDT Spray By James Bond 1 /2.7 /4.2 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
+                &lt;p&gt;007 Cologne by James Bond, A mysterious and alluring new cologne inspired by ian flemingâ€™s fictional character james bond is to be released in 2012. The launching of this secretive menâ€™s cologne is scheduled to coincide with the 50th anniversary of the first debut of the original film, as well as the release of the newest james bond movie. While there is yet no scoop on what this new cologne will smell like, it is certain to be as enchanting, alluring and mysterious as its inspiration.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/M471110.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/00742MBON.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -623,7 +596,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -635,18 +607,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -657,10 +624,16 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>10 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/M471110.jpg</t>
+    <t>4.2 oz Eau De Toilette Spray</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/00742MBON.jpg</t>
+  </si>
+  <si>
+    <t>4711 Perfume By Muelhens Deodorant Spray (Unisex)</t>
+  </si>
+  <si>
+    <t>100% Genuine 4711 Deodorant Spray (Unisex) By Muelhens 5 Oz</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -710,18 +683,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 Deodorant Spray (Unisex) By Muelhens 5 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
+                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C13M.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/58258W.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -793,7 +766,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -805,18 +777,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -827,10 +794,28 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>13.5 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/471C13M.jpg</t>
+    <t>Muelhens</t>
+  </si>
+  <si>
+    <t>Deodorant Spray (Unisex)</t>
+  </si>
+  <si>
+    <t>5 oz Deodorant Spray</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/58258W.jpg</t>
+  </si>
+  <si>
+    <t>Perfume for Women</t>
+  </si>
+  <si>
+    <t>Perfume</t>
+  </si>
+  <si>
+    <t>4711 Cologne By Muelhens Eau De Cologne (Unisex)</t>
+  </si>
+  <si>
+    <t>100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -880,7 +865,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -891,7 +876,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU4711-27M.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C17.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -963,7 +948,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -975,18 +959,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -997,10 +976,13 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>27 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/AU4711-27M.jpg</t>
+    <t>Eau De Cologne (Unisex)</t>
+  </si>
+  <si>
+    <t>1.7 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/471C17.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -1050,7 +1032,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1061,7 +1043,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/88562M.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/M471110.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -1133,7 +1115,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -1145,18 +1126,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1167,10 +1143,10 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>3.3 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/88562M.jpg</t>
+    <t>10 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/M471110.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -1220,7 +1196,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1231,7 +1207,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471T5M.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C13M.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -1303,7 +1279,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -1315,18 +1290,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1337,10 +1307,10 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>5 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/471T5M.jpg</t>
+    <t>13.5 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/471C13M.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -1390,7 +1360,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1401,7 +1371,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU4711-67M.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU4711-27M.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -1473,7 +1443,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -1485,18 +1454,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1507,13 +1471,10 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>6.8 oz Eau De Cologne</t>
-  </si>
-  <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/AU4711-67M.jpg</t>
-  </si>
-  <si>
-    <t>4711 Perfume By Muelhens Eau De Cologne (Unisex)</t>
+    <t>27 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/AU4711-27M.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -1563,18 +1524,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
+                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C17W.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/88562M.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -1646,7 +1607,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -1658,18 +1618,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1680,7 +1635,10 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/471C17W.jpg</t>
+    <t>3.3 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/88562M.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -1730,18 +1688,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
+                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/W471110.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471T5M.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -1813,7 +1771,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -1825,18 +1782,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -1847,7 +1799,10 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/W471110.jpg</t>
+    <t>5 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/471T5M.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -1897,18 +1852,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
+                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C13.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU4711-67M.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -1980,7 +1935,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -1992,18 +1946,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2014,7 +1963,13 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/471C13.jpg</t>
+    <t>6.8 oz Eau De Cologne</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/AU4711-67M.jpg</t>
+  </si>
+  <si>
+    <t>4711 Perfume By Muelhens Eau De Cologne (Unisex)</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -2064,7 +2019,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2075,7 +2030,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU4711-27W.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C17W.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -2147,7 +2102,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -2159,18 +2113,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2181,7 +2130,7 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/AU4711-27W.jpg</t>
+    <t>https://img.fragrancex.com/images/products/SKU/large/471C17W.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -2231,7 +2180,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2242,7 +2191,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/88562W.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/W471110.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -2314,7 +2263,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -2326,18 +2274,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2348,7 +2291,7 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/88562W.jpg</t>
+    <t>https://img.fragrancex.com/images/products/SKU/large/W471110.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -2398,7 +2341,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2409,7 +2352,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471T5W.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471C13.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -2481,7 +2424,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -2493,18 +2435,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2515,7 +2452,7 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/471T5W.jpg</t>
+    <t>https://img.fragrancex.com/images/products/SKU/large/471C13.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -2565,7 +2502,7 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2576,7 +2513,7 @@
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU471167W.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU4711-27W.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -2648,7 +2585,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -2660,18 +2596,13 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
-                    &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -2682,13 +2613,7 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>https://img.fragrancex.com/images/products/SKU/large/AU471167W.jpg</t>
-  </si>
-  <si>
-    <t>4711 Cologne By Muelhens Eau De Cologne (Unisex-Unboxed)</t>
-  </si>
-  <si>
-    <t>100% Genuine 4711 EDC (Unisex-Unboxed) By Muelhens 13.5 Oz</t>
+    <t>https://img.fragrancex.com/images/products/SKU/large/AU4711-27W.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;style&gt;
@@ -2738,18 +2663,18 @@
         &lt;div class="row"&gt;
             &lt;font size="8"&gt;
                 &lt;b&gt;
-                    100% Genuine 4711 EDC (Unisex-Unboxed) By Muelhens 13.5 Oz
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
                 &lt;/b&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row"&gt;
             &lt;font size="5"&gt;
                 &lt;h3&gt;Product description: &lt;/h3&gt;
-                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
+                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
             &lt;/font&gt;
         &lt;/div&gt;
         &lt;div class="row back" align="center"&gt;
-            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471113U.jpg"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/88562W.jpg"&gt;
         &lt;/div&gt;
         &lt;div class="row back"&gt;
             &lt;font size="5"&gt;
@@ -2821,7 +2746,6 @@
             &lt;font size="5"&gt;
                 &lt;h3&gt;Shipping Information &lt;/h3&gt;
                 &lt;ul style="list-style-type:disc"&gt;
-                    &lt;li&gt;&lt;b&gt;International Shipping:&lt;/b&gt; $10 &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
                     &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
                 &lt;/ul&gt;
@@ -2833,18 +2757,502 @@
                 &lt;ul style="list-style-type:disc"&gt;
                     &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
                     &lt;li&gt;
-                        6 month Warranty (SoundCue Offers warranty for internal electronic components with the receipt as proof
-                        of purchase. Warranty does not cover misuse, physical damage, and or liquid damage.)
-                    &lt;/li&gt;
-                    &lt;li&gt;
                         Our number one priority is to provide you with fast shipping,
-                        great service and authentic products. Please do not hesitade to
+                        great service and authentic products. Please do not hesitate to
                         contact us if there are any issues.
                     &lt;/li&gt;
                     &lt;li&gt;Refunds are available. &lt;/li&gt;
                     &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
-                    &lt;li&gt;Item must be in its original case before a return is acepted.&lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
+                &lt;/ul&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row" align="center"&gt;
+            &lt;font size="6"&gt;&lt;b&gt; Thank You For Visiting Us!! &lt;/b&gt;&lt;/font&gt; &lt;br /&gt;
+        &lt;/div&gt;
+    &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/88562W.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;style&gt;
+.row {
+	margin: 10px 0px;
+}
+.row:after {
+	content: "";
+	display: table;
+	clear: both;
+}
+.left{
+	float:left;
+}
+.right{
+	float:right;
+}
+h1{
+	padding: 1%;
+}
+.imgTitle {
+	height: 200;
+	width: 300;
+	align: center:
+}
+.imgSunglasses{
+	height: 350;
+	width: 400;
+}
+.back{
+	background: #3385ff;
+	padding: 1%;
+}
+div{
+	..border-style:dotted;
+	..border-width:1px;
+}
+&lt;/style&gt;
+&lt;div class="row back" align="center"&gt;
+    &lt;img class="imgTitle" src="https://thugcode.com/EA/ebay/Phil/phil.png"&gt;
+&lt;/div&gt;
+&lt;div class="row " align="center"&gt;
+    &lt;div class="row back"&gt;
+        &lt;div class="row" align="center"&gt;
+            &lt;font size="8"&gt;&lt;b&gt; eBay Phil's Boutique &lt;/b&gt;&lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="8"&gt;
+                &lt;b&gt;
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
+                &lt;/b&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Product description: &lt;/h3&gt;
+                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row back" align="center"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471T5W.jpg"&gt;
+        &lt;/div&gt;
+        &lt;div class="row back"&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Just What Is the Difference Between Perfume, Eau de Parfum, Eau de Toilette, Cologne, and Testers?&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Shopping for fragrance can be confusing at best, or overwhelming at worst. Not only are there top notes, middle notes,
+                    and bottom notes, but whole classes of scents. What’s more, once you’ve decided on a scent, another decision must be made:
+                    perfume, eau de parfum, eau de toilette or cologne?
+                &lt;/p&gt;
+                &lt;p&gt;
+                    Fragrances are available in perfume, eau de parfum, eau de toilette, or cologne form. The main differentiating factor of these
+                    is the concentration of aromatic compounds in a solvent – that is, how much fragrance is in the formula’s composition. The more
+                    actual perfume concentrate it contains, the longer the scent will last on your skin, and the more expensive the product. Following
+                    is a breakdown of these categories.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Perfume&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Perfume, also referred to as perfume extract, is the most concentrated formulation, and is usually the most expensive. It contains
+                    15-30% aromatic compounds. Due to its high amount of aromatic compounds, it also tends to last the longest when applied to the skin.
+                    It is usually sold in small bottles of 1 ounce or less.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Eau de Parfum&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de parfum, also called eau de perfume, is the next most concentrated formula, and one of the most popular purchases. It
+                    consists of 10-15% aromatic compounds.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Eau de Toilette&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de toilette is also a popular choice, and is less expensive than the perfume or parfum formulations, although its scent will
+                    not last as long when applied to the skin. Eau de toilette contains 5-20% aromatic compounds.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Cologne, or Eau de Cologne&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de Cologne originated in Cologne, Germany. Today, it is a generic term that defines a class of scented formulations by its
+                    typical concentration of about 2-5%. Cologne products are available for either men or women, and are sometimes mistaken for aftershave,
+                    which is actually a formula containing moisturizer, an antiseptic agent, and perfume. In addition, aftershave can be a gel, lotion, or liquid.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Tester&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Testers are even more discounted than the fancy boxed versions and are great if you don't have a need for the fancy box. Testers are 100%
+                    authentic, fresh and completely full just like the original fragrance, however they are meant for the counter in a department store. Testers
+                    often come in a plain white box but sometimes they do not have a cap or a box. The savings on the packaging means you save even more!
+                &lt;/p&gt;
+                &lt;p&gt;
+                    For any perfume concentration, be sure to keep the bottle tightly sealed and stored in a cool, dry place away from windows or direct sunlight
+                    or heat sources to maximize its shelf life. For best results, store opened bottles inside their boxes. Fragrances usually last three years
+                    from the date they were manufactured.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;What is the difference between a splash and a spray?&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    There is absolutely no difference in the fragrance. The difference is in the method of application only. However, a spray bottle, being sealed
+                    all the time, may actually have a longer shelf life. Making the decision between spray and splash is entirely a matter of personal preference.
+                &lt;/p&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Shipping Information &lt;/h3&gt;
+                &lt;ul style="list-style-type:disc"&gt;
+                    &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
+                    &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
+                &lt;/ul&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Return policy &lt;/h3&gt;
+                &lt;ul style="list-style-type:disc"&gt;
+                    &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
+                    &lt;li&gt;
+                        Our number one priority is to provide you with fast shipping,
+                        great service and authentic products. Please do not hesitate to
+                        contact us if there are any issues.
                     &lt;/li&gt;
+                    &lt;li&gt;Refunds are available. &lt;/li&gt;
+                    &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
+                &lt;/ul&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row" align="center"&gt;
+            &lt;font size="6"&gt;&lt;b&gt; Thank You For Visiting Us!! &lt;/b&gt;&lt;/font&gt; &lt;br /&gt;
+        &lt;/div&gt;
+    &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/471T5W.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;style&gt;
+.row {
+	margin: 10px 0px;
+}
+.row:after {
+	content: "";
+	display: table;
+	clear: both;
+}
+.left{
+	float:left;
+}
+.right{
+	float:right;
+}
+h1{
+	padding: 1%;
+}
+.imgTitle {
+	height: 200;
+	width: 300;
+	align: center:
+}
+.imgSunglasses{
+	height: 350;
+	width: 400;
+}
+.back{
+	background: #3385ff;
+	padding: 1%;
+}
+div{
+	..border-style:dotted;
+	..border-width:1px;
+}
+&lt;/style&gt;
+&lt;div class="row back" align="center"&gt;
+    &lt;img class="imgTitle" src="https://thugcode.com/EA/ebay/Phil/phil.png"&gt;
+&lt;/div&gt;
+&lt;div class="row " align="center"&gt;
+    &lt;div class="row back"&gt;
+        &lt;div class="row" align="center"&gt;
+            &lt;font size="8"&gt;&lt;b&gt; eBay Phil's Boutique &lt;/b&gt;&lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="8"&gt;
+                &lt;b&gt;
+                    100% Genuine 4711 EDC (Unisex) By Muelhens 1.7 /10 /13.5 /27 /3.3 /6.8 /6.8 Oz
+                &lt;/b&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Product description: &lt;/h3&gt;
+                &lt;p&gt;4711 Perfume by Muelhens, Launched by the design house of muelhens in 1772, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of citrus oils lemon &amp; orange, light floral rose, and sandalwood oil. It is recommended for daytime wear.&lt;/p&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row back" align="center"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/AU471167W.jpg"&gt;
+        &lt;/div&gt;
+        &lt;div class="row back"&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Just What Is the Difference Between Perfume, Eau de Parfum, Eau de Toilette, Cologne, and Testers?&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Shopping for fragrance can be confusing at best, or overwhelming at worst. Not only are there top notes, middle notes,
+                    and bottom notes, but whole classes of scents. What’s more, once you’ve decided on a scent, another decision must be made:
+                    perfume, eau de parfum, eau de toilette or cologne?
+                &lt;/p&gt;
+                &lt;p&gt;
+                    Fragrances are available in perfume, eau de parfum, eau de toilette, or cologne form. The main differentiating factor of these
+                    is the concentration of aromatic compounds in a solvent – that is, how much fragrance is in the formula’s composition. The more
+                    actual perfume concentrate it contains, the longer the scent will last on your skin, and the more expensive the product. Following
+                    is a breakdown of these categories.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Perfume&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Perfume, also referred to as perfume extract, is the most concentrated formulation, and is usually the most expensive. It contains
+                    15-30% aromatic compounds. Due to its high amount of aromatic compounds, it also tends to last the longest when applied to the skin.
+                    It is usually sold in small bottles of 1 ounce or less.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Eau de Parfum&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de parfum, also called eau de perfume, is the next most concentrated formula, and one of the most popular purchases. It
+                    consists of 10-15% aromatic compounds.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Eau de Toilette&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de toilette is also a popular choice, and is less expensive than the perfume or parfum formulations, although its scent will
+                    not last as long when applied to the skin. Eau de toilette contains 5-20% aromatic compounds.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Cologne, or Eau de Cologne&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de Cologne originated in Cologne, Germany. Today, it is a generic term that defines a class of scented formulations by its
+                    typical concentration of about 2-5%. Cologne products are available for either men or women, and are sometimes mistaken for aftershave,
+                    which is actually a formula containing moisturizer, an antiseptic agent, and perfume. In addition, aftershave can be a gel, lotion, or liquid.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Tester&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Testers are even more discounted than the fancy boxed versions and are great if you don't have a need for the fancy box. Testers are 100%
+                    authentic, fresh and completely full just like the original fragrance, however they are meant for the counter in a department store. Testers
+                    often come in a plain white box but sometimes they do not have a cap or a box. The savings on the packaging means you save even more!
+                &lt;/p&gt;
+                &lt;p&gt;
+                    For any perfume concentration, be sure to keep the bottle tightly sealed and stored in a cool, dry place away from windows or direct sunlight
+                    or heat sources to maximize its shelf life. For best results, store opened bottles inside their boxes. Fragrances usually last three years
+                    from the date they were manufactured.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;What is the difference between a splash and a spray?&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    There is absolutely no difference in the fragrance. The difference is in the method of application only. However, a spray bottle, being sealed
+                    all the time, may actually have a longer shelf life. Making the decision between spray and splash is entirely a matter of personal preference.
+                &lt;/p&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Shipping Information &lt;/h3&gt;
+                &lt;ul style="list-style-type:disc"&gt;
+                    &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
+                    &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
+                &lt;/ul&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Return policy &lt;/h3&gt;
+                &lt;ul style="list-style-type:disc"&gt;
+                    &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
+                    &lt;li&gt;
+                        Our number one priority is to provide you with fast shipping,
+                        great service and authentic products. Please do not hesitate to
+                        contact us if there are any issues.
+                    &lt;/li&gt;
+                    &lt;li&gt;Refunds are available. &lt;/li&gt;
+                    &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
+                &lt;/ul&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row" align="center"&gt;
+            &lt;font size="6"&gt;&lt;b&gt; Thank You For Visiting Us!! &lt;/b&gt;&lt;/font&gt; &lt;br /&gt;
+        &lt;/div&gt;
+    &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>https://img.fragrancex.com/images/products/SKU/large/AU471167W.jpg</t>
+  </si>
+  <si>
+    <t>4711 Cologne By Muelhens Eau De Cologne (Unisex-Unboxed)</t>
+  </si>
+  <si>
+    <t>100% Genuine 4711 EDC (Unisex-Unboxed) By Muelhens 13.5 Oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;style&gt;
+.row {
+	margin: 10px 0px;
+}
+.row:after {
+	content: "";
+	display: table;
+	clear: both;
+}
+.left{
+	float:left;
+}
+.right{
+	float:right;
+}
+h1{
+	padding: 1%;
+}
+.imgTitle {
+	height: 200;
+	width: 300;
+	align: center:
+}
+.imgSunglasses{
+	height: 350;
+	width: 400;
+}
+.back{
+	background: #3385ff;
+	padding: 1%;
+}
+div{
+	..border-style:dotted;
+	..border-width:1px;
+}
+&lt;/style&gt;
+&lt;div class="row back" align="center"&gt;
+    &lt;img class="imgTitle" src="https://thugcode.com/EA/ebay/Phil/phil.png"&gt;
+&lt;/div&gt;
+&lt;div class="row " align="center"&gt;
+    &lt;div class="row back"&gt;
+        &lt;div class="row" align="center"&gt;
+            &lt;font size="8"&gt;&lt;b&gt; eBay Phil's Boutique &lt;/b&gt;&lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="8"&gt;
+                &lt;b&gt;
+                    100% Genuine 4711 EDC (Unisex-Unboxed) By Muelhens 13.5 Oz
+                &lt;/b&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Product description: &lt;/h3&gt;
+                &lt;p&gt;4711 Cologne by Muelhens, Created by the design house of muelhens in 1792, 4711 is classified as a refined, fruity fragrance. This unisex scent possesses a blend of sandalwood oils, citrus fruits, oranges, lemons, and grapefruit.&lt;/p&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row back" align="center"&gt;
+            &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/471113U.jpg"&gt;
+        &lt;/div&gt;
+        &lt;div class="row back"&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Just What Is the Difference Between Perfume, Eau de Parfum, Eau de Toilette, Cologne, and Testers?&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Shopping for fragrance can be confusing at best, or overwhelming at worst. Not only are there top notes, middle notes,
+                    and bottom notes, but whole classes of scents. What’s more, once you’ve decided on a scent, another decision must be made:
+                    perfume, eau de parfum, eau de toilette or cologne?
+                &lt;/p&gt;
+                &lt;p&gt;
+                    Fragrances are available in perfume, eau de parfum, eau de toilette, or cologne form. The main differentiating factor of these
+                    is the concentration of aromatic compounds in a solvent – that is, how much fragrance is in the formula’s composition. The more
+                    actual perfume concentrate it contains, the longer the scent will last on your skin, and the more expensive the product. Following
+                    is a breakdown of these categories.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Perfume&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Perfume, also referred to as perfume extract, is the most concentrated formulation, and is usually the most expensive. It contains
+                    15-30% aromatic compounds. Due to its high amount of aromatic compounds, it also tends to last the longest when applied to the skin.
+                    It is usually sold in small bottles of 1 ounce or less.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Eau de Parfum&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de parfum, also called eau de perfume, is the next most concentrated formula, and one of the most popular purchases. It
+                    consists of 10-15% aromatic compounds.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Eau de Toilette&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de toilette is also a popular choice, and is less expensive than the perfume or parfum formulations, although its scent will
+                    not last as long when applied to the skin. Eau de toilette contains 5-20% aromatic compounds.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Cologne, or Eau de Cologne&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Eau de Cologne originated in Cologne, Germany. Today, it is a generic term that defines a class of scented formulations by its
+                    typical concentration of about 2-5%. Cologne products are available for either men or women, and are sometimes mistaken for aftershave,
+                    which is actually a formula containing moisturizer, an antiseptic agent, and perfume. In addition, aftershave can be a gel, lotion, or liquid.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;Tester&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    Testers are even more discounted than the fancy boxed versions and are great if you don't have a need for the fancy box. Testers are 100%
+                    authentic, fresh and completely full just like the original fragrance, however they are meant for the counter in a department store. Testers
+                    often come in a plain white box but sometimes they do not have a cap or a box. The savings on the packaging means you save even more!
+                &lt;/p&gt;
+                &lt;p&gt;
+                    For any perfume concentration, be sure to keep the bottle tightly sealed and stored in a cool, dry place away from windows or direct sunlight
+                    or heat sources to maximize its shelf life. For best results, store opened bottles inside their boxes. Fragrances usually last three years
+                    from the date they were manufactured.
+                &lt;/p&gt;
+            &lt;/font&gt;
+            &lt;font size="5"&gt;
+                &lt;font size="8"&gt;&lt;b&gt;What is the difference between a splash and a spray?&lt;/b&gt;&lt;/font&gt;
+                &lt;p&gt;
+                    There is absolutely no difference in the fragrance. The difference is in the method of application only. However, a spray bottle, being sealed
+                    all the time, may actually have a longer shelf life. Making the decision between spray and splash is entirely a matter of personal preference.
+                &lt;/p&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Shipping Information &lt;/h3&gt;
+                &lt;ul style="list-style-type:disc"&gt;
+                    &lt;li&gt;&lt;b&gt;USA Shipping:&lt;/b&gt; Free Shipping &lt;/li&gt;
+                    &lt;li&gt;&lt;b&gt;Handling Time:&lt;/b&gt; 1 Business day after clear payment &lt;/li&gt;
+                &lt;/ul&gt;
+            &lt;/font&gt;
+        &lt;/div&gt;
+        &lt;div class="row"&gt;
+            &lt;font size="5"&gt;
+                &lt;h3&gt;Return policy &lt;/h3&gt;
+                &lt;ul style="list-style-type:disc"&gt;
+                    &lt;li&gt;100% Customer Satisfaction Guaranteed!! &lt;/li&gt;
+                    &lt;li&gt;
+                        Our number one priority is to provide you with fast shipping,
+                        great service and authentic products. Please do not hesitate to
+                        contact us if there are any issues.
+                    &lt;/li&gt;
+                    &lt;li&gt;Refunds are available. &lt;/li&gt;
+                    &lt;li&gt;Refunds shipping will be paid by the buyer. &lt;/li&gt;
+                    &lt;li&gt;Item must be in its original case and sealed before a return is accepted.&lt;/li&gt;
                 &lt;/ul&gt;
             &lt;/font&gt;
         &lt;/div&gt;
@@ -3214,10 +3622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEEF1B7-81D4-4526-9648-DAB22F146F36}">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,10 +3751,10 @@
         <v>33</v>
       </c>
       <c r="M2" s="0">
-        <v>416473</v>
+        <v>539808</v>
       </c>
       <c r="N2" s="0">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>34</v>
@@ -3362,9 +3770,6 @@
       </c>
       <c r="S2" s="1">
         <v>24.28</v>
-      </c>
-      <c r="T2" s="0">
-        <v>15</v>
       </c>
       <c r="U2" s="0" t="b">
         <v>1</v>
@@ -3384,19 +3789,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F3" s="0" t="b">
         <v>1</v>
@@ -3405,13 +3810,13 @@
         <v>32</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M3" s="0">
-        <v>416452</v>
+        <v>482296</v>
       </c>
       <c r="N3" s="0">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>34</v>
@@ -3426,10 +3831,7 @@
         <v>36</v>
       </c>
       <c r="S3" s="1">
-        <v>16.07</v>
-      </c>
-      <c r="T3" s="0">
-        <v>15.5</v>
+        <v>49.12</v>
       </c>
       <c r="U3" s="0" t="b">
         <v>1</v>
@@ -3438,30 +3840,30 @@
         <v>0</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="b">
         <v>1</v>
@@ -3470,13 +3872,13 @@
         <v>32</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M4" s="0">
-        <v>416457</v>
+        <v>511013</v>
       </c>
       <c r="N4" s="0">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>34</v>
@@ -3491,10 +3893,7 @@
         <v>36</v>
       </c>
       <c r="S4" s="1">
-        <v>41.41</v>
-      </c>
-      <c r="T4" s="0">
-        <v>35</v>
+        <v>68.54</v>
       </c>
       <c r="U4" s="0" t="b">
         <v>1</v>
@@ -3503,30 +3902,30 @@
         <v>0</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AA4" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F5" s="0" t="b">
         <v>1</v>
@@ -3535,13 +3934,13 @@
         <v>32</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M5" s="0">
-        <v>416467</v>
+        <v>416473</v>
       </c>
       <c r="N5" s="0">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>34</v>
@@ -3556,10 +3955,10 @@
         <v>36</v>
       </c>
       <c r="S5" s="1">
-        <v>49.12</v>
+        <v>24.28</v>
       </c>
       <c r="T5" s="0">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="U5" s="0" t="b">
         <v>1</v>
@@ -3568,30 +3967,30 @@
         <v>0</v>
       </c>
       <c r="X5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z5" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="Z5" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="AA5" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F6" s="0" t="b">
         <v>1</v>
@@ -3600,13 +3999,13 @@
         <v>32</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M6" s="0">
-        <v>416445</v>
+        <v>416452</v>
       </c>
       <c r="N6" s="0">
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="O6" s="0" t="s">
         <v>34</v>
@@ -3621,10 +4020,10 @@
         <v>36</v>
       </c>
       <c r="S6" s="1">
-        <v>78.54</v>
+        <v>16.07</v>
       </c>
       <c r="T6" s="0">
-        <v>50</v>
+        <v>15.5</v>
       </c>
       <c r="U6" s="0" t="b">
         <v>1</v>
@@ -3633,30 +4032,30 @@
         <v>0</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F7" s="0" t="b">
         <v>1</v>
@@ -3665,13 +4064,13 @@
         <v>32</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M7" s="0">
-        <v>416463</v>
+        <v>416457</v>
       </c>
       <c r="N7" s="0">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>34</v>
@@ -3686,10 +4085,10 @@
         <v>36</v>
       </c>
       <c r="S7" s="1">
-        <v>20.36</v>
+        <v>41.41</v>
       </c>
       <c r="T7" s="0">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="U7" s="0" t="b">
         <v>1</v>
@@ -3698,30 +4097,30 @@
         <v>0</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F8" s="0" t="b">
         <v>1</v>
@@ -3730,13 +4129,13 @@
         <v>32</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M8" s="0">
-        <v>416454</v>
+        <v>416467</v>
       </c>
       <c r="N8" s="0">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="O8" s="0" t="s">
         <v>34</v>
@@ -3751,10 +4150,10 @@
         <v>36</v>
       </c>
       <c r="S8" s="1">
-        <v>23.73</v>
+        <v>49.12</v>
       </c>
       <c r="T8" s="0">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="U8" s="0" t="b">
         <v>1</v>
@@ -3763,30 +4162,30 @@
         <v>0</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F9" s="0" t="b">
         <v>1</v>
@@ -3795,13 +4194,13 @@
         <v>32</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M9" s="0">
-        <v>416446</v>
+        <v>416445</v>
       </c>
       <c r="N9" s="0">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="O9" s="0" t="s">
         <v>34</v>
@@ -3816,10 +4215,10 @@
         <v>36</v>
       </c>
       <c r="S9" s="1">
-        <v>27.13</v>
+        <v>78.54</v>
       </c>
       <c r="T9" s="0">
-        <v>28.5</v>
+        <v>50</v>
       </c>
       <c r="U9" s="0" t="b">
         <v>1</v>
@@ -3828,30 +4227,30 @@
         <v>0</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F10" s="0" t="b">
         <v>1</v>
@@ -3860,13 +4259,13 @@
         <v>32</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="M10" s="0">
-        <v>416477</v>
+        <v>416463</v>
       </c>
       <c r="N10" s="0">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="O10" s="0" t="s">
         <v>34</v>
@@ -3881,10 +4280,10 @@
         <v>36</v>
       </c>
       <c r="S10" s="1">
-        <v>16.07</v>
+        <v>20.36</v>
       </c>
       <c r="T10" s="0">
-        <v>10.5</v>
+        <v>20</v>
       </c>
       <c r="U10" s="0" t="b">
         <v>1</v>
@@ -3893,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Z10" s="0" t="s">
         <v>38</v>
@@ -3904,19 +4303,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F11" s="0" t="b">
         <v>1</v>
@@ -3925,13 +4324,13 @@
         <v>32</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="M11" s="0">
-        <v>416479</v>
+        <v>416454</v>
       </c>
       <c r="N11" s="0">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>34</v>
@@ -3946,7 +4345,7 @@
         <v>36</v>
       </c>
       <c r="S11" s="1">
-        <v>41.41</v>
+        <v>23.73</v>
       </c>
       <c r="T11" s="0">
         <v>30</v>
@@ -3958,7 +4357,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Z11" s="0" t="s">
         <v>38</v>
@@ -3969,19 +4368,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F12" s="0" t="b">
         <v>1</v>
@@ -3990,13 +4389,13 @@
         <v>32</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="M12" s="0">
-        <v>416487</v>
+        <v>416446</v>
       </c>
       <c r="N12" s="0">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="O12" s="0" t="s">
         <v>34</v>
@@ -4011,10 +4410,10 @@
         <v>36</v>
       </c>
       <c r="S12" s="1">
-        <v>49.12</v>
+        <v>27.13</v>
       </c>
       <c r="T12" s="0">
-        <v>40</v>
+        <v>28.5</v>
       </c>
       <c r="U12" s="0" t="b">
         <v>1</v>
@@ -4023,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="Z12" s="0" t="s">
         <v>38</v>
@@ -4034,19 +4433,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="b">
         <v>1</v>
@@ -4055,13 +4454,13 @@
         <v>32</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M13" s="0">
-        <v>416470</v>
+        <v>416477</v>
       </c>
       <c r="N13" s="0">
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="O13" s="0" t="s">
         <v>34</v>
@@ -4076,10 +4475,10 @@
         <v>36</v>
       </c>
       <c r="S13" s="1">
-        <v>78.54</v>
+        <v>16.07</v>
       </c>
       <c r="T13" s="0">
-        <v>50</v>
+        <v>10.5</v>
       </c>
       <c r="U13" s="0" t="b">
         <v>1</v>
@@ -4088,30 +4487,30 @@
         <v>0</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AA13" s="0" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F14" s="0" t="b">
         <v>1</v>
@@ -4120,13 +4519,13 @@
         <v>32</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M14" s="0">
-        <v>416469</v>
+        <v>416479</v>
       </c>
       <c r="N14" s="0">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="O14" s="0" t="s">
         <v>34</v>
@@ -4141,10 +4540,10 @@
         <v>36</v>
       </c>
       <c r="S14" s="1">
-        <v>20.36</v>
+        <v>41.41</v>
       </c>
       <c r="T14" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U14" s="0" t="b">
         <v>1</v>
@@ -4153,30 +4552,30 @@
         <v>0</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AA14" s="0" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F15" s="0" t="b">
         <v>1</v>
@@ -4185,13 +4584,13 @@
         <v>32</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M15" s="0">
-        <v>416476</v>
+        <v>416487</v>
       </c>
       <c r="N15" s="0">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="O15" s="0" t="s">
         <v>34</v>
@@ -4206,10 +4605,10 @@
         <v>36</v>
       </c>
       <c r="S15" s="1">
-        <v>24.58</v>
+        <v>49.12</v>
       </c>
       <c r="T15" s="0">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="U15" s="0" t="b">
         <v>1</v>
@@ -4218,30 +4617,30 @@
         <v>0</v>
       </c>
       <c r="X15" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="Z15" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AA15" s="0" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F16" s="0" t="b">
         <v>1</v>
@@ -4250,13 +4649,13 @@
         <v>32</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M16" s="0">
-        <v>416468</v>
+        <v>416470</v>
       </c>
       <c r="N16" s="0">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="O16" s="0" t="s">
         <v>34</v>
@@ -4271,10 +4670,10 @@
         <v>36</v>
       </c>
       <c r="S16" s="1">
-        <v>27.13</v>
+        <v>78.54</v>
       </c>
       <c r="T16" s="0">
-        <v>28.5</v>
+        <v>50</v>
       </c>
       <c r="U16" s="0" t="b">
         <v>1</v>
@@ -4283,30 +4682,30 @@
         <v>0</v>
       </c>
       <c r="X16" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Z16" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AA16" s="0" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="F17" s="0" t="b">
         <v>1</v>
@@ -4315,13 +4714,13 @@
         <v>32</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="M17" s="0">
-        <v>454162</v>
+        <v>416469</v>
       </c>
       <c r="N17" s="0">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>34</v>
@@ -4336,7 +4735,10 @@
         <v>36</v>
       </c>
       <c r="S17" s="1">
-        <v>48.55</v>
+        <v>20.36</v>
+      </c>
+      <c r="T17" s="0">
+        <v>20</v>
       </c>
       <c r="U17" s="0" t="b">
         <v>1</v>
@@ -4345,13 +4747,205 @@
         <v>0</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="Z17" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="AA17" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" s="0">
+        <v>416476</v>
+      </c>
+      <c r="N18" s="0">
+        <v>500</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="0">
+        <v>500</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" s="1">
+        <v>24.58</v>
+      </c>
+      <c r="T18" s="0">
+        <v>30</v>
+      </c>
+      <c r="U18" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="V18" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA18" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="0">
+        <v>416468</v>
+      </c>
+      <c r="N19" s="0">
+        <v>600</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" s="0">
+        <v>500</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" s="1">
+        <v>27.13</v>
+      </c>
+      <c r="T19" s="0">
+        <v>28.5</v>
+      </c>
+      <c r="U19" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="V19" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA19" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="0">
+        <v>454162</v>
+      </c>
+      <c r="N20" s="0">
+        <v>800</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" s="0">
+        <v>500</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20" s="1">
+        <v>48.55</v>
+      </c>
+      <c r="U20" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="V20" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA20" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>